<commit_message>
Added code to support least-distance character classification. Added code to remove OCR mistakes caused by similar characters (e.g. "1" and "l") Added support for multi-threaded least-distance classification.
</commit_message>
<xml_diff>
--- a/Documentation/Test Results/Recognition Rates.xlsx
+++ b/Documentation/Test Results/Recognition Rates.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Recognition Rate</t>
   </si>
@@ -42,6 +42,42 @@
   </si>
   <si>
     <t>170/243</t>
+  </si>
+  <si>
+    <t>After spell check</t>
+  </si>
+  <si>
+    <t>128/149 (85.9%)</t>
+  </si>
+  <si>
+    <t>211/243</t>
+  </si>
+  <si>
+    <t>Neural Network</t>
+  </si>
+  <si>
+    <t>Classification Method</t>
+  </si>
+  <si>
+    <t>Least Distance</t>
+  </si>
+  <si>
+    <t>230/243 (94.7%)</t>
+  </si>
+  <si>
+    <t>*** 20x20 raw img input w/ sets 2 and 3</t>
+  </si>
+  <si>
+    <t>224/243</t>
+  </si>
+  <si>
+    <t>224/243 (92.2%)</t>
+  </si>
+  <si>
+    <t>83/117</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -363,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -374,9 +410,11 @@
     <col min="1" max="1" width="17.88671875" customWidth="1"/>
     <col min="2" max="2" width="15.77734375" customWidth="1"/>
     <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -386,8 +424,14 @@
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -397,10 +441,65 @@
       <c r="C2" s="2">
         <v>0.7</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added code to use multiple classification algorithms for the same image. In other words, the translation will be "proofread" by different algorithms and improved if needed.
</commit_message>
<xml_diff>
--- a/Documentation/Test Results/Recognition Rates.xlsx
+++ b/Documentation/Test Results/Recognition Rates.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Recognition Rate</t>
   </si>
@@ -78,6 +78,21 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>82/92</t>
+  </si>
+  <si>
+    <t>82/92 (89.1%)</t>
+  </si>
+  <si>
+    <t>88/92</t>
+  </si>
+  <si>
+    <t>90/92 (97.8%)</t>
+  </si>
+  <si>
+    <t>Average Recognition</t>
   </si>
 </sst>
 </file>
@@ -399,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,6 +517,49 @@
         <v>11</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17">
+        <f>AVERAGE(C2:C7)</f>
+        <v>0.84116666666666662</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished optimization of trained font recognition. Added training data and documentation of test results.
</commit_message>
<xml_diff>
--- a/Documentation/Test Results/Recognition Rates.xlsx
+++ b/Documentation/Test Results/Recognition Rates.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>Recognition Rate</t>
   </si>
@@ -41,21 +41,12 @@
     <t>Times New Roman</t>
   </si>
   <si>
-    <t>170/243</t>
-  </si>
-  <si>
     <t>After spell check</t>
   </si>
   <si>
-    <t>128/149 (85.9%)</t>
-  </si>
-  <si>
     <t>211/243</t>
   </si>
   <si>
-    <t>Neural Network</t>
-  </si>
-  <si>
     <t>Classification Method</t>
   </si>
   <si>
@@ -93,13 +84,28 @@
   </si>
   <si>
     <t>Average Recognition</t>
+  </si>
+  <si>
+    <t>144/167</t>
+  </si>
+  <si>
+    <t>159/167</t>
+  </si>
+  <si>
+    <t>208/243</t>
+  </si>
+  <si>
+    <t>AFTER OPTIMIZATION (Size invariant)</t>
+  </si>
+  <si>
+    <t>*** 212/243 after factoring in unavoidable OCR mistakes, such as the difference between "I" and "l" (lower L and Upper i)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,13 +113,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -125,17 +143,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -417,7 +440,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,47 +463,34 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2">
         <v>0.86799999999999999</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -488,16 +498,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2">
         <v>0.92200000000000004</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -505,16 +515,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2">
         <v>0.70899999999999996</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -522,16 +532,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2">
         <v>0.89100000000000001</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -539,28 +549,76 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2">
         <v>0.95699999999999996</v>
       </c>
       <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.86199999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
         <v>21</v>
       </c>
-      <c r="E7" t="s">
-        <v>11</v>
+      <c r="C11" s="2">
+        <v>0.95199999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17">
-        <f>AVERAGE(C2:C7)</f>
-        <v>0.84116666666666662</v>
+        <v>19</v>
+      </c>
+      <c r="C17" s="2">
+        <f>AVERAGE(C2:C12)</f>
+        <v>0.87712500000000004</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A9:E9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>

</xml_diff>